<commit_message>
[Engine] [Renderer/Editor] Render Debug Grid, Add depth write to rt
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3C9E40-455C-4747-918F-04BF14058477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D6CAED-D85E-4F7D-B2EC-60498682735B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="2010" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +233,10 @@
   </si>
   <si>
     <t>2023.11.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forward Pass实现基础的blin phong光照</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -695,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -850,6 +854,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:H4" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[Engine] [Core] refactor InputManager is static class
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D6CAED-D85E-4F7D-B2EC-60498682735B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EEA9D4-02AF-46E7-9188-48A831BC4981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="2010" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -237,6 +237,22 @@
   </si>
   <si>
     <t>Forward Pass实现基础的blin phong光照</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将Input调整为全局单例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -699,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -809,21 +825,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -863,6 +882,23 @@
       </c>
       <c r="C8" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Core] fix inspector draw, add input mouse wheel delta
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EEA9D4-02AF-46E7-9188-48A831BC4981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D071ED-5D37-4633-AEDA-41650D20CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7380" yWindow="2010" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -249,6 +249,10 @@
   </si>
   <si>
     <t>将Input调整为全局单例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -718,7 +722,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -884,21 +888,24 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>46</v>
+      <c r="F9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Render] refactor RenderCamera，Add RendererPath
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D071ED-5D37-4633-AEDA-41650D20CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B3D68-5C5A-42A7-BDC0-46667AE37BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="2010" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -257,6 +257,34 @@
   </si>
   <si>
     <t>2023.11.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增RendererPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>切换渲染路径，抽象Scene、Game等渲染路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整RenderCameraController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -719,10 +747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -815,18 +843,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -906,6 +943,46 @@
       </c>
       <c r="G9" s="2" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Render] refactor cameraController
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1B3D68-5C5A-42A7-BDC0-46667AE37BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735657C4-1239-42F7-8A13-BB24CFCB3814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="4605" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,7 +284,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2023.11.11</t>
+    <t>2023.11.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renderer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整Material</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据重构的管线，修改Material反射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Editor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整理资源目录结构</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -627,7 +651,7 @@
   <dimension ref="A3:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -747,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -914,15 +938,21 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -968,21 +998,55 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Render] commit shader reflection
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735657C4-1239-42F7-8A13-BB24CFCB3814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D219A309-0309-4E76-B416-171670EB1AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="4605" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -774,7 +774,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -921,21 +921,24 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>46</v>
+      <c r="F7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[Engine] [Editor] fixed sceneView viewport size
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D219A309-0309-4E76-B416-171670EB1AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929EF9E3-7BCC-4327-AFD8-16A2A0DE857D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="4605" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10320" yWindow="1605" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -309,6 +309,26 @@
   </si>
   <si>
     <t>整理资源目录结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.11.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sean Duan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Renderer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Material新增默认标准材质</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进行中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -771,10 +791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1018,27 +1038,30 @@
         <v>64</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>46</v>
+      <c r="F12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1050,6 +1073,23 @@
       </c>
       <c r="C13" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Editor] adopt hierarchy
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E5385C-18D7-40D0-9670-4048423D201C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2165F047-FB8A-4230-87B4-3F784291B7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2460" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4440" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t>调整 Forward Pass  绘制阴影</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asset Flow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资产管理, 各种资源的支持，如：模型、贴图、材质、场景、预制体等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整模型导入，支持层级结构和预制体序列化机制</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,11 +412,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -685,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D17"/>
+  <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -769,33 +780,41 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -808,10 +827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1126,15 +1145,26 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Engine] [Editor] adopt asset dir
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2165F047-FB8A-4230-87B4-3F784291B7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AFDEC7-B707-442C-98EA-D06697FFB21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4440" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11415" yWindow="3930" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -357,6 +357,10 @@
   </si>
   <si>
     <t>调整模型导入，支持层级结构和预制体序列化机制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -830,7 +834,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1100,15 +1104,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[Engine] [UI] Add RectTransform、UICanvas
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FAFE74-175E-48CD-9BFC-10599065C01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217FEC9-AF80-4E15-9209-7C5FEE65B7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -474,6 +474,13 @@
   <si>
     <t>实现GameView的Renderer Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hitmoti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sakupinera</t>
   </si>
 </sst>
 </file>
@@ -947,7 +954,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1360,76 +1367,83 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>100</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Engine] [Renderer] Added LinesPass
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BB4AA5-B3EF-4765-BB75-E709EF63A571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196846B4-9E09-45B8-B4E9-27825A512E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="3390" windowWidth="27135" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
-    <sheet name="Roadmap" sheetId="3" r:id="rId2"/>
+    <sheet name="Roadmap(Doing)" sheetId="4" r:id="rId2"/>
+    <sheet name="Roadmap(Complete)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Roadmap!$B$1:$H$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Roadmap(Complete)'!$B$1:$H$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="160">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -516,6 +517,152 @@
   </si>
   <si>
     <t>2023.1.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现基础的PBR着色器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现天空盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sean Duan</t>
+  </si>
+  <si>
+    <t>实现ProjectHubPanel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.4.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化MaterialEditor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.4.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接入Profiler</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化平行光Shadow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.4.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增GridPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增IconPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增LinesPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化渲染层Buffer的缓存机制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>充分缓存Descriptor, 避免频繁排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化可渲染对象排序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增透明物体渲染</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Engine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>补充代码注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增SelectedAssetViewPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.3.31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增Prefab机制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.3.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整RendererPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.3.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.2.28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.2.26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.1.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构Grid的绘制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增SkyBoxPass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.3.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化PBR着色器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PBR新增IBL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hitmoti</t>
+  </si>
+  <si>
+    <t>原野</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优化贴图导入流程</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -986,11 +1133,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1AA135-B7E3-48D0-8271-04DFC02FCBDA}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="33.375" customWidth="1"/>
+    <col min="4" max="4" width="40.625" customWidth="1"/>
+    <col min="5" max="5" width="13.75" customWidth="1"/>
+    <col min="8" max="8" width="24.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1136,6 +1465,9 @@
       <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1174,7 +1506,7 @@
         <v>86</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1388,19 +1720,16 @@
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>38</v>
@@ -1414,135 +1743,363 @@
         <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="G21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="F22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" t="s">
-        <v>109</v>
-      </c>
-    </row>
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="B1:H4" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[Engine] [Standalone] Updated Standalone
</commit_message>
<xml_diff>
--- a/Design/Roadmap.xlsx
+++ b/Design/Roadmap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\LitchiEngineGit\LitchiEngineGithub\LitchiEngine\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Res\LitchiEngine\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196846B4-9E09-45B8-B4E9-27825A512E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DC90D6-A412-4882-8393-C970616A9E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="路线图总览" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="166">
   <si>
     <t>渲染</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -663,6 +663,30 @@
   </si>
   <si>
     <t>优化贴图导入流程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.5.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调整Camera序列化结构和编辑器绘制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.5.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增SceneView内嵌套绘制参数面板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.5.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.6.3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -718,11 +742,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1134,11 +1157,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1AA135-B7E3-48D0-8271-04DFC02FCBDA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1222,89 +1245,81 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>140</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1316,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2099,7 +2114,57 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:H4" xr:uid="{81F02DA2-DE12-4AB0-9E71-817FBFDF18D7}"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>